<commit_message>
[Update] API, frontend pages
</commit_message>
<xml_diff>
--- a/wms_backend/static/mapping.xlsx
+++ b/wms_backend/static/mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngaip\Desktop\WMS\wms_backend\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D4F0CF-BDAA-49C2-BCE6-0A8B81C1AE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F35721-B2D8-47F1-A03D-7F5E0D78FFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>XT</t>
   </si>
@@ -46,9 +46,6 @@
     <t>000003</t>
   </si>
   <si>
-    <t>000004</t>
-  </si>
-  <si>
     <t>PosCode</t>
   </si>
   <si>
@@ -98,12 +95,6 @@
   </si>
   <si>
     <t>D4</t>
-  </si>
-  <si>
-    <t>000005</t>
-  </si>
-  <si>
-    <t>000006</t>
   </si>
 </sst>
 </file>
@@ -490,14 +481,14 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -511,7 +502,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -525,7 +516,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -539,7 +530,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -553,7 +544,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -567,10 +558,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -581,10 +572,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -595,10 +586,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -609,10 +600,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -623,10 +614,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -637,10 +628,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -651,10 +642,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -665,10 +656,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -679,10 +670,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -693,10 +684,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
@@ -707,10 +698,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -721,10 +712,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>

</xml_diff>